<commit_message>
Add compare label function.
</commit_message>
<xml_diff>
--- a/demo/AXG4A_Spec_Demo.xlsx
+++ b/demo/AXG4A_Spec_Demo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Menu</t>
   </si>
@@ -119,26 +119,6 @@
   </si>
   <si>
     <t>Level 6</t>
-  </si>
-  <si>
-    <t>Change PV map</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Change SV map</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Change TV map</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Change QV map</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Method</t>
-    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -512,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,58 +807,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add source code for getting register log and report.
</commit_message>
<xml_diff>
--- a/demo/AXG4A_Spec_Demo.xlsx
+++ b/demo/AXG4A_Spec_Demo.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
-    <sheet name="Label" sheetId="1" r:id="rId1"/>
+    <sheet name="Spec" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>Menu</t>
   </si>
@@ -119,13 +119,75 @@
   </si>
   <si>
     <t>Level 6</t>
+  </si>
+  <si>
+    <t>High/Low alarm configuration</t>
+  </si>
+  <si>
+    <t>Low alarm</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Low low alarm</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>High alarm</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>High high alarm</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Hi/Lo alarm hysteresis</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Maintenance root menu</t>
+  </si>
+  <si>
+    <t>R/W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>7g</t>
+  </si>
+  <si>
+    <t>Min.</t>
+  </si>
+  <si>
+    <t>Max.</t>
+  </si>
+  <si>
+    <t>2.0f</t>
+  </si>
+  <si>
+    <t>UINT</t>
+  </si>
+  <si>
+    <t>ENUM</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +213,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -166,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,17 +265,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +294,22 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -492,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -506,305 +606,652 @@
     <col min="5" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="J1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4" t="s">
-        <v>3</v>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="7"/>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>